<commit_message>
Cambios varios modulo siif, reporte programas, dat y tra
</commit_message>
<xml_diff>
--- a/src/main/resources/plantillas/nomina/Producto_Nomina_Programas.xlsx
+++ b/src/main/resources/plantillas/nomina/Producto_Nomina_Programas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>R. F. C.</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>PROSPERA PAQUETE BASICO</t>
+  </si>
+  <si>
+    <t>NO.</t>
   </si>
 </sst>
 </file>
@@ -260,22 +263,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>79376</xdr:colOff>
+      <xdr:colOff>190501</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>285751</xdr:rowOff>
+      <xdr:rowOff>79374</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>79375</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>31751</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Imagen 1" descr="C:\Users\Infraestructura\Downloads\SESA.jpg">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AE960556-00EB-4253-BCCE-5C4F0FFCF07C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE960556-00EB-4253-BCCE-5C4F0FFCF07C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -296,8 +299,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="79376" y="285751"/>
-          <a:ext cx="1619249" cy="1492250"/>
+          <a:off x="190501" y="79374"/>
+          <a:ext cx="2698749" cy="1317626"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -579,23 +582,22 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
-    <col min="6" max="6" width="23.42578125" customWidth="1"/>
-    <col min="7" max="7" width="21" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" style="6" customWidth="1"/>
-    <col min="10" max="10" width="24.28515625" style="6" customWidth="1"/>
-    <col min="11" max="11" width="22.85546875" style="6" customWidth="1"/>
-    <col min="12" max="12" width="34.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="6" customWidth="1"/>
+    <col min="11" max="11" width="24.28515625" style="6" customWidth="1"/>
+    <col min="12" max="12" width="22.85546875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="7" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
@@ -695,61 +697,63 @@
       <c r="L6" s="12"/>
     </row>
     <row r="7" spans="1:12" s="7" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="9"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="10"/>
       <c r="H7" s="8"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="11"/>
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
     </row>
     <row r="8" spans="1:12" s="1" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="I8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="J8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="K8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="L8" s="5" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A6:L6"/>
+    <mergeCell ref="A5:L5"/>
     <mergeCell ref="A4:L4"/>
     <mergeCell ref="A3:L3"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A5:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="22" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>

</xml_diff>